<commit_message>
Update: Stability added to Greek computation using volatility surface.
</commit_message>
<xml_diff>
--- a/Booking/GasCall.xlsx
+++ b/Booking/GasCall.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CYTech Student\PycharmProjects\Quantitative_Finance\Booking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{221E41BD-7A09-4245-B1EF-C6DBCE8B8CC5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{060C286C-5F8C-48F3-A22A-363F1877A694}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -132,13 +132,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <b/>
@@ -154,7 +159,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -177,13 +182,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -856,58 +882,58 @@
   <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
     </row>
@@ -931,25 +957,25 @@
         <v>20</v>
       </c>
       <c r="G2">
-        <v>3.6180000305175781</v>
+        <v>3.7479999065399099</v>
       </c>
       <c r="H2">
-        <v>53032.143891429492</v>
+        <v>65597.031814058006</v>
       </c>
       <c r="I2">
-        <v>16.70967840379285</v>
+        <v>20.903222791610229</v>
       </c>
       <c r="M2">
-        <v>9.5197868398755325</v>
+        <v>9.7910342034213116</v>
       </c>
       <c r="N2">
-        <v>2.8562886775773682</v>
+        <v>1.3917007724018049</v>
       </c>
       <c r="O2">
-        <v>4.6322870095316651E-3</v>
+        <v>2.4147576271893452E-3</v>
       </c>
       <c r="P2">
-        <v>-3.7071392166067127E-2</v>
+        <v>-2.337068811595587E-2</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -972,25 +998,25 @@
         <v>20</v>
       </c>
       <c r="G3">
-        <v>3.6180000305175781</v>
+        <v>3.747999906539917</v>
       </c>
       <c r="H3">
-        <v>-28108.696990645421</v>
+        <v>-40659.437609753477</v>
       </c>
       <c r="I3">
-        <v>1.9154938173965741</v>
+        <v>5.5774621560540139</v>
       </c>
       <c r="M3">
-        <v>-8.9875649795274626</v>
+        <v>-10.899471748775371</v>
       </c>
       <c r="N3">
-        <v>-15.510279870234459</v>
+        <v>-13.143873390575321</v>
       </c>
       <c r="O3">
-        <v>-2.6896546791332909E-2</v>
+        <v>-2.3980766795439479E-2</v>
       </c>
       <c r="P3">
-        <v>0.18879827066018981</v>
+        <v>0.1679892072422873</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -1007,10 +1033,10 @@
         <v>20</v>
       </c>
       <c r="G4">
-        <v>3.6180000305175781</v>
+        <v>3.747999906539917</v>
       </c>
       <c r="H4">
-        <v>-36180.000305175781</v>
+        <v>-37479.99906539917</v>
       </c>
       <c r="M4">
         <v>-1</v>
@@ -1024,28 +1050,28 @@
         <v>34</v>
       </c>
       <c r="G5">
-        <v>3.6180000305175781</v>
+        <v>3.747999906539917</v>
       </c>
       <c r="H5">
-        <v>-11256.553404391711</v>
+        <v>-12542.404861094639</v>
       </c>
       <c r="J5">
         <v>10950</v>
       </c>
       <c r="K5">
-        <v>-306.55340439170692</v>
+        <v>-1592.4048610946411</v>
       </c>
       <c r="M5">
-        <v>-0.46777813965192999</v>
+        <v>-2.1084375453540569</v>
       </c>
       <c r="N5">
-        <v>-12.65399119265709</v>
+        <v>-11.752172618173519</v>
       </c>
       <c r="O5">
-        <v>-2.226425978180124E-2</v>
+        <v>-2.156600916825013E-2</v>
       </c>
       <c r="P5">
-        <v>0.15172687849412261</v>
+        <v>0.14461851912633139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>